<commit_message>
results all omic with explainable models
</commit_message>
<xml_diff>
--- a/Results_all_omics.xlsx
+++ b/Results_all_omics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastien.delandtshe\PycharmProjects\DeepOncoAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85F1509-9A99-4183-BF05-09CCB7CE269F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC46E211-A467-4E75-8818-348F8D45DB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="1470" windowWidth="27315" windowHeight="16140" activeTab="2" xr2:uid="{AB31E162-962E-479B-8A46-7E7DA2E68AD3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{AB31E162-962E-479B-8A46-7E7DA2E68AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="177">
   <si>
     <t>17-AAG</t>
   </si>
@@ -169,9 +169,6 @@
     <t>TNFa; JAK-STAT</t>
   </si>
   <si>
-    <t>NQO1</t>
-  </si>
-  <si>
     <t>Bax; XBP1; Caspase7-cleaved; Gab2</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>MAPK-PI3K</t>
   </si>
   <si>
-    <t>IFI27; PREX2</t>
-  </si>
-  <si>
     <t>Shc_pY317; HER2_pY1248</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>GABA; beta-alanine; DHAP/G3P; a-glycerophosphate</t>
   </si>
   <si>
-    <t>miR-222; miR-34a; miR-130a; miR-222; let-7c; miR-497; miR-582-5p; miR-223</t>
-  </si>
-  <si>
     <t xml:space="preserve">ETV4; SPRY2; RP11-93B14.5; ETV5; ZNF502; SPRY1; TOR4A; CMTM7; DUSP6; </t>
   </si>
   <si>
@@ -560,15 +551,45 @@
   </si>
   <si>
     <t>Bax; VAV1; Annexin1; p21</t>
+  </si>
+  <si>
+    <t>miR-222; miR-34a; miR-130a; let-7c; miR-497; miR-582-5p; miR-223</t>
+  </si>
+  <si>
+    <t>NQO1; MB21D1; SLC16A3</t>
+  </si>
+  <si>
+    <t>Explainable</t>
+  </si>
+  <si>
+    <t>Diff expl-RNA</t>
+  </si>
+  <si>
+    <t>IFI27; PREX2; PLAGL1; GSTT1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -859,7 +880,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -921,6 +942,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,7 +1000,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> integration versus single</a:t>
+              <a:t> integration versus single omic versus explainable</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2513,6 +2536,193 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-94DE-4981-962E-A781648ED54D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>plot!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Explainable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>plot!$A$2:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>PD-0325901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AZD6244</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paclitaxel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Panobinostat</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Irinotecan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Erlotinib</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Lapatinib</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>TAE684</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PD-0332991</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17-AAG</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>RAF265</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>TKI258</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Nilotinib</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>PF2341066</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ZD-6474</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>AEW541</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>PLX4720</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>L-685458</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Sorafenib</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>AZD0530</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>PHA-665752</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Nutlin3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>LBW242</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>plot!$J$2:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.751</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.60499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.59899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.57199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.64500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.61099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.71899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.56699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.56399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.64500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7AF9-4123-85BD-FB065AA5EB82}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3265,7 +3475,7 @@
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
@@ -4329,15 +4539,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116FF058-1CDD-40C9-8FFD-6CCCF68842D5}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
@@ -4345,7 +4556,7 @@
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4373,18 +4584,24 @@
       <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
         <v>0.873</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="21">
         <v>0.874</v>
       </c>
       <c r="D2">
@@ -4405,16 +4622,23 @@
       <c r="I2">
         <v>0.67500000000000004</v>
       </c>
-      <c r="K2">
+      <c r="J2">
+        <v>0.81</v>
+      </c>
+      <c r="L2">
         <f>B2-(MAX(C2:I2))</f>
         <v>-1.0000000000000009E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>J2-C2</f>
+        <v>-6.3999999999999946E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="21">
         <v>0.872</v>
       </c>
       <c r="C3">
@@ -4438,19 +4662,26 @@
       <c r="I3">
         <v>0.51400000000000001</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K24" si="0">B3-(MAX(C3:I3))</f>
+      <c r="J3">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L24" si="0">B3-(MAX(C3:I3))</f>
         <v>2.200000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f t="shared" ref="M3:M24" si="1">J3-C3</f>
+        <v>-1.6999999999999904E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
         <v>0.84299999999999997</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="21">
         <v>0.86099999999999999</v>
       </c>
       <c r="D4">
@@ -4471,16 +4702,23 @@
       <c r="I4">
         <v>0.69299999999999995</v>
       </c>
-      <c r="K4">
+      <c r="J4">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="0"/>
         <v>-1.8000000000000016E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>-1.9000000000000017E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="21">
         <v>0.82299999999999995</v>
       </c>
       <c r="C5">
@@ -4504,19 +4742,26 @@
       <c r="I5">
         <v>0.69899999999999995</v>
       </c>
-      <c r="K5">
+      <c r="J5">
+        <v>0.751</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="0"/>
         <v>1.2999999999999901E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>-5.9000000000000052E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0.80400000000000005</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="21">
         <v>0.83899999999999997</v>
       </c>
       <c r="D6">
@@ -4537,16 +4782,23 @@
       <c r="I6">
         <v>0.72599999999999998</v>
       </c>
-      <c r="K6">
+      <c r="J6">
+        <v>0.89</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="0"/>
         <v>-3.499999999999992E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000045E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="21">
         <v>0.79700000000000004</v>
       </c>
       <c r="C7">
@@ -4570,16 +4822,23 @@
       <c r="I7">
         <v>0.61499999999999999</v>
       </c>
-      <c r="K7">
+      <c r="J7">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="0"/>
         <v>8.0000000000000071E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>-7.900000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="21">
         <v>0.79300000000000004</v>
       </c>
       <c r="C8">
@@ -4603,12 +4862,19 @@
       <c r="I8">
         <v>0.56299999999999994</v>
       </c>
-      <c r="K8">
+      <c r="J8">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="0"/>
         <v>1.2000000000000011E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>-6.9999999999999951E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4624,7 +4890,7 @@
       <c r="E9">
         <v>0.48299999999999998</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="21">
         <v>0.72599999999999998</v>
       </c>
       <c r="G9">
@@ -4636,16 +4902,23 @@
       <c r="I9">
         <v>0.58199999999999996</v>
       </c>
-      <c r="K9">
+      <c r="J9">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="0"/>
         <v>-3.0000000000000027E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>3.9000000000000035E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="21">
         <v>0.71899999999999997</v>
       </c>
       <c r="C10">
@@ -4669,19 +4942,26 @@
       <c r="I10">
         <v>0.65400000000000003</v>
       </c>
-      <c r="K10">
+      <c r="J10">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="0"/>
         <v>2.300000000000002E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>6.4000000000000057E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11">
         <v>0.71699999999999997</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="21">
         <v>0.71799999999999997</v>
       </c>
       <c r="D11">
@@ -4702,16 +4982,23 @@
       <c r="I11">
         <v>0.55900000000000005</v>
       </c>
-      <c r="K11">
+      <c r="J11">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="0"/>
         <v>-1.0000000000000009E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>-6.6999999999999948E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="21">
         <v>0.71099999999999997</v>
       </c>
       <c r="C12">
@@ -4735,16 +5022,23 @@
       <c r="I12">
         <v>0.60799999999999998</v>
       </c>
-      <c r="K12">
+      <c r="J12">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="0"/>
         <v>1.100000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>-6.1999999999999944E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="21">
         <v>0.71099999999999997</v>
       </c>
       <c r="C13">
@@ -4768,12 +5062,19 @@
       <c r="I13">
         <v>0.48899999999999999</v>
       </c>
-      <c r="K13">
+      <c r="J13">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="0"/>
         <v>6.0999999999999943E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4798,15 +5099,22 @@
       <c r="H14">
         <v>0.68300000000000005</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="21">
         <v>0.70599999999999996</v>
       </c>
-      <c r="K14">
+      <c r="J14" s="22">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="0"/>
         <v>-8.0000000000000071E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>-4.3000000000000038E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -4825,7 +5133,7 @@
       <c r="F15">
         <v>0.67800000000000005</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="21">
         <v>0.69299999999999995</v>
       </c>
       <c r="H15">
@@ -4834,12 +5142,19 @@
       <c r="I15">
         <v>0.57199999999999995</v>
       </c>
-      <c r="K15">
+      <c r="J15">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="0"/>
         <v>-1.19999999999999E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>-7.5000000000000067E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -4855,7 +5170,7 @@
       <c r="E16">
         <v>0.495</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="21">
         <v>0.67700000000000005</v>
       </c>
       <c r="G16">
@@ -4867,12 +5182,19 @@
       <c r="I16">
         <v>0.53400000000000003</v>
       </c>
-      <c r="K16">
+      <c r="J16">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="0"/>
         <v>-3.0000000000000027E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>-1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -4891,7 +5213,7 @@
       <c r="F17">
         <v>0.56100000000000005</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="21">
         <v>0.63800000000000001</v>
       </c>
       <c r="H17">
@@ -4900,16 +5222,23 @@
       <c r="I17">
         <v>0.55200000000000005</v>
       </c>
-      <c r="K17">
+      <c r="J17">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="0"/>
         <v>-4.0000000000000036E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="21">
         <v>0.627</v>
       </c>
       <c r="C18">
@@ -4933,19 +5262,26 @@
       <c r="I18">
         <v>0.51900000000000002</v>
       </c>
-      <c r="K18">
+      <c r="J18">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="0"/>
         <v>1.7000000000000015E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000071E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19">
         <v>0.61499999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="21">
         <v>0.63600000000000001</v>
       </c>
       <c r="D19">
@@ -4966,19 +5302,26 @@
       <c r="I19">
         <v>0.60399999999999998</v>
       </c>
-      <c r="K19">
+      <c r="J19">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="0"/>
         <v>-2.1000000000000019E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>8.2999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0.59199999999999997</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="21">
         <v>0.6</v>
       </c>
       <c r="D20">
@@ -4999,12 +5342,19 @@
       <c r="I20">
         <v>0.495</v>
       </c>
-      <c r="K20">
+      <c r="J20">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="0"/>
         <v>-8.0000000000000071E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>-3.3000000000000029E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -5029,15 +5379,22 @@
       <c r="H21">
         <v>0.497</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="21">
         <v>0.59799999999999998</v>
       </c>
-      <c r="K21">
+      <c r="J21" s="22">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="0"/>
         <v>-7.0000000000000062E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>-2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5050,7 +5407,7 @@
       <c r="D22">
         <v>0.52100000000000002</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="21">
         <v>0.60299999999999998</v>
       </c>
       <c r="F22">
@@ -5065,12 +5422,19 @@
       <c r="I22">
         <v>0.505</v>
       </c>
-      <c r="K22">
+      <c r="J22">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="0"/>
         <v>-2.5000000000000022E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>-5.0000000000000044E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -5086,7 +5450,7 @@
       <c r="E23">
         <v>0.42099999999999999</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="21">
         <v>0.68500000000000005</v>
       </c>
       <c r="G23">
@@ -5098,12 +5462,19 @@
       <c r="I23">
         <v>0.501</v>
       </c>
-      <c r="K23">
+      <c r="J23">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="0"/>
         <v>-0.1140000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>0.14500000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -5113,7 +5484,7 @@
       <c r="C24">
         <v>0.49</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="21">
         <v>0.55600000000000005</v>
       </c>
       <c r="E24">
@@ -5131,16 +5502,35 @@
       <c r="I24">
         <v>0.48499999999999999</v>
       </c>
-      <c r="K24">
+      <c r="J24">
+        <v>0.5</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="0"/>
         <v>-4.7000000000000042E-2</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000009E-2</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I27">
     <sortCondition descending="1" ref="B2:B27"/>
   </sortState>
-  <conditionalFormatting sqref="K2:K24 K26">
+  <conditionalFormatting sqref="L2:L24 L26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5153,7 +5543,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5161,8 +5552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109902AE-C79C-4B5F-A611-595D07D30130}">
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5177,7 +5568,7 @@
     <row r="1" spans="2:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>33</v>
@@ -5209,25 +5600,25 @@
         <v>0.873</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="I3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5238,25 +5629,25 @@
         <v>0.872</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>62</v>
-      </c>
       <c r="G4" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5267,25 +5658,25 @@
         <v>0.84299999999999997</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E5" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>108</v>
-      </c>
       <c r="I5" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5296,25 +5687,25 @@
         <v>0.82299999999999995</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="H6" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5325,25 +5716,25 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>78</v>
-      </c>
       <c r="I7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5354,25 +5745,25 @@
         <v>0.79700000000000004</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="J8" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5383,25 +5774,25 @@
         <v>0.79300000000000004</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="G9" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5412,25 +5803,25 @@
         <v>0.72299999999999998</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F10" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>158</v>
-      </c>
       <c r="I10" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5441,25 +5832,25 @@
         <v>0.71899999999999997</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5470,7 +5861,7 @@
         <v>0.71699999999999997</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>40</v>
@@ -5479,10 +5870,10 @@
         <v>42</v>
       </c>
       <c r="G12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>43</v>
@@ -5499,25 +5890,25 @@
         <v>0.71099999999999997</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F13" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>146</v>
-      </c>
       <c r="I13" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5528,25 +5919,25 @@
         <v>0.71099999999999997</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>162</v>
-      </c>
       <c r="J14" s="15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5557,25 +5948,25 @@
         <v>0.69799999999999995</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="H15" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5586,25 +5977,25 @@
         <v>0.68100000000000005</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5615,25 +6006,25 @@
         <v>0.67400000000000004</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5644,25 +6035,25 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="H18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="J18" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5673,25 +6064,25 @@
         <v>0.627</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F19" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>140</v>
-      </c>
       <c r="I19" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5702,25 +6093,25 @@
         <v>0.61499999999999999</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="G20" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>83</v>
-      </c>
       <c r="H20" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5731,25 +6122,25 @@
         <v>0.59199999999999997</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E21" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>150</v>
-      </c>
       <c r="J21" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5760,25 +6151,25 @@
         <v>0.59099999999999997</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="I22" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5789,25 +6180,25 @@
         <v>0.57799999999999996</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E23" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>134</v>
-      </c>
       <c r="H23" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5818,25 +6209,25 @@
         <v>0.57099999999999995</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E24" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="G24" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>103</v>
-      </c>
       <c r="I24" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5847,25 +6238,25 @@
         <v>0.50900000000000001</v>
       </c>
       <c r="D25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>93</v>
-      </c>
       <c r="I25" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>